<commit_message>
atualizado lista 3ds II
</commit_message>
<xml_diff>
--- a/Lista Nintendo 3DS.xlsx
+++ b/Lista Nintendo 3DS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="65">
   <si>
     <t>Nome</t>
   </si>
@@ -121,82 +121,94 @@
     <t>não</t>
   </si>
   <si>
+    <t>Monster Hunter 4 Ultimate</t>
+  </si>
+  <si>
+    <t>Shinobi</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda - Majoras Mask</t>
+  </si>
+  <si>
+    <t>Xenoblade Chronicles</t>
+  </si>
+  <si>
+    <t>Tekken 3d - Prime Edition</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country Returns</t>
+  </si>
+  <si>
+    <t>Tales of Abyss</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts - Dream Drop Distance</t>
+  </si>
+  <si>
+    <t>Need for Speed - The Run</t>
+  </si>
+  <si>
+    <t>Final Fantasy Explorers</t>
+  </si>
+  <si>
+    <t>Pokemon Sun</t>
+  </si>
+  <si>
+    <t>Fire Emblem Fates - Special Edition</t>
+  </si>
+  <si>
+    <t>Kirby Planet Robobot</t>
+  </si>
+  <si>
+    <t>Heroes of Ruin</t>
+  </si>
+  <si>
+    <t>Lbx Little Battlers Experience</t>
+  </si>
+  <si>
+    <t>Mario Sports Superstars</t>
+  </si>
+  <si>
+    <t>Yugioh - Saikyo Card Battle</t>
+  </si>
+  <si>
+    <t>Naruto Shipudden 3ds</t>
+  </si>
+  <si>
+    <t>Batman - Arkhan Origins Blackgate</t>
+  </si>
+  <si>
+    <t>Medabots</t>
+  </si>
+  <si>
+    <t>Iron Fall - Invasion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex Troppers </t>
+  </si>
+  <si>
+    <t>Azure Striker Gunvolt 2</t>
+  </si>
+  <si>
+    <t>Mario Tennis</t>
+  </si>
+  <si>
+    <t>Tank Troopers</t>
+  </si>
+  <si>
+    <t>Hakuoki - Memories of the Shinsengumi</t>
+  </si>
+  <si>
+    <t>Inazuma Eleven Go</t>
+  </si>
+  <si>
     <t>Monster Hunter Stories</t>
   </si>
   <si>
-    <t>Monster Hunter 4 Ultimate</t>
-  </si>
-  <si>
-    <t>Shinobi</t>
-  </si>
-  <si>
-    <t>The Legend of Zelda - Majoras Mask</t>
-  </si>
-  <si>
-    <t>Xenoblade Chronicles</t>
-  </si>
-  <si>
-    <t>Tekken 3d - Prime Edition</t>
-  </si>
-  <si>
-    <t>Donkey Kong Country Returns</t>
-  </si>
-  <si>
-    <t>Tales of Abyss</t>
-  </si>
-  <si>
-    <t>Kingdom Hearts - Dream Drop Distance</t>
-  </si>
-  <si>
-    <t>Need for Speed - The Run</t>
-  </si>
-  <si>
-    <t>Final Fantasy Explorers</t>
-  </si>
-  <si>
-    <t>Pokemon Sun</t>
-  </si>
-  <si>
-    <t>Fire Emblem Fates - Special Edition</t>
-  </si>
-  <si>
-    <t>Kirby Planet Robobot</t>
-  </si>
-  <si>
-    <t>Heroes of Ruin</t>
-  </si>
-  <si>
-    <t>Lbx Little Battlers Experience</t>
-  </si>
-  <si>
-    <t>Mario Sports Superstars</t>
-  </si>
-  <si>
-    <t>Yugioh - Saikyo Card Battle</t>
-  </si>
-  <si>
-    <t>Naruto Shipudden 3ds</t>
-  </si>
-  <si>
-    <t>Batman - Arkhan Origins Blackgate</t>
-  </si>
-  <si>
-    <t>Medabots</t>
-  </si>
-  <si>
-    <t>Iron Fall - Invasion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ex Troppers </t>
-  </si>
-  <si>
-    <t>Azure Striker Gunvolt 2</t>
-  </si>
-  <si>
-    <t>Mario Tennis</t>
-  </si>
-  <si>
-    <t>Tank Troopers</t>
+    <t>Cars 2</t>
+  </si>
+  <si>
+    <t>Angry Birds - Star Wars</t>
   </si>
 </sst>
 </file>
@@ -204,10 +216,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;* #,##0_-;\-&quot;R$&quot;* #,##0_-;_-&quot;R$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -226,6 +238,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,15 +284,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,10 +313,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -277,11 +367,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,83 +381,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -385,187 +397,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -579,13 +591,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,24 +617,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -640,24 +638,29 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,153 +679,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1205,10 +1217,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A50" sqref="$A50:$XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -1564,8 +1576,8 @@
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>34</v>
+      <c r="C33" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1575,8 +1587,8 @@
       <c r="B34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>34</v>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1586,8 +1598,8 @@
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>34</v>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1597,8 +1609,8 @@
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>4</v>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1608,8 +1620,8 @@
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>34</v>
+      <c r="C37" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1652,8 +1664,8 @@
       <c r="B41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>34</v>
+      <c r="C41" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1663,8 +1675,8 @@
       <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>34</v>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1718,8 +1730,8 @@
       <c r="B47" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>34</v>
+      <c r="C47" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1740,30 +1752,30 @@
       <c r="B49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>4</v>
+      <c r="C49" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
+      <c r="A50" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>34</v>
+      <c r="C50" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>34</v>
+      <c r="C51" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1773,8 +1785,8 @@
       <c r="B52" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>4</v>
+      <c r="C52" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1806,8 +1818,8 @@
       <c r="B55" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>34</v>
+      <c r="C55" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1841,6 +1853,50 @@
       </c>
       <c r="C58" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>